<commit_message>
Cuaderno de estudio Tema 9
Cuaderno de estudio y mapa conceptual listos para revisión de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion09/ESCALETA_ MA_09_09_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion09/ESCALETA_ MA_09_09_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion09\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="7920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="248">
   <si>
     <t>Asignatura</t>
   </si>
@@ -555,9 +560,6 @@
     <t>Identifica el método de demostración</t>
   </si>
   <si>
-    <t>Actividad para determinar qué métod de demostración se aplica para comprobar una proposición</t>
-  </si>
-  <si>
     <t>Presentar demostraciones sencillas en las que sea fácil identificar si corresponde al método directo, indirecto, contraejemplo. Esas mismas alternativas son las posibles respuestas</t>
   </si>
   <si>
@@ -621,9 +623,6 @@
     <t xml:space="preserve">Presentar imágenes que muestren los criterios de semejanza, en las imágenes mostrar pares de triángulos que cumplan uno de los criterios señalados </t>
   </si>
   <si>
-    <t>Interactivo para reconocer los criterios de semejnaza de triángulos</t>
-  </si>
-  <si>
     <t>Aplica los criterios de semejanza de triángulos</t>
   </si>
   <si>
@@ -657,15 +656,9 @@
     <t>Presentar el procedimiento para la construcción de polígonos semejantes a partir del trabajo con regla y compás desde las homotecias. Construir recurso off line</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las longitudes proporcionales</t>
-  </si>
-  <si>
     <t>Actividad para aplicar razones trigonometricas y calcular datos desconocidos en un triángulo</t>
   </si>
   <si>
-    <t>Actividades sobre Las longitudes proporcionales</t>
-  </si>
-  <si>
     <t>Proyecto  para construir polígonos semejantes con regla y compás, aplicando conceptos relacionados como las homotecias</t>
   </si>
   <si>
@@ -696,9 +689,6 @@
     <t>La semejanza de triángulos</t>
   </si>
   <si>
-    <t>Las longitudes proporcionales</t>
-  </si>
-  <si>
     <t xml:space="preserve">Interactivo para profundizar en las estrategias para realizar demostraciones </t>
   </si>
   <si>
@@ -708,15 +698,9 @@
     <t>Ejercicios que permiten la aplicación del teorema de Tales para calcular distancias</t>
   </si>
   <si>
-    <t>Interactivo que explica la relación entre los tripangulos rectángulos y las razones trigonométricas</t>
-  </si>
-  <si>
     <t>Construir fichas de tal manera que se explica en qué consiste cada método y dar ejemplos sencillos que permitan la fácil comprensión de cada uno de los métodos. Incluir, método directo, indirecto, contraejemplo</t>
   </si>
   <si>
-    <t>Identifca hipótesis y tesis</t>
-  </si>
-  <si>
     <t xml:space="preserve">La semejanza de polígonos </t>
   </si>
   <si>
@@ -760,6 +744,30 @@
   </si>
   <si>
     <t>Recurso M101AP-01</t>
+  </si>
+  <si>
+    <t>Actividad para determinar el método de demostración que se aplica para comprobar una proposición</t>
+  </si>
+  <si>
+    <t>Identifica hipótesis y tesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completa demostraciones indirectas </t>
+  </si>
+  <si>
+    <t>Interactivo para reconocer los criterios de semejanza de triángulos</t>
+  </si>
+  <si>
+    <t>La semejanza de triángulos rectángulos</t>
+  </si>
+  <si>
+    <t>Interactivo que explica la relación entre los triángulos rectángulos y las razones trigonométricas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La semejanza de triángulos rectángulos</t>
+  </si>
+  <si>
+    <t>Actividad sobre La semejanza de triángulos rectángulos</t>
   </si>
 </sst>
 </file>
@@ -945,70 +953,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1086,6 +1034,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,7 +1154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1181,7 +1189,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1393,1911 +1401,1919 @@
   <dimension ref="A1:U79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="A15:XFD15"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.7109375" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="30.7109375" style="18"/>
-    <col min="5" max="5" width="24.5703125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="52" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" style="18"/>
-    <col min="8" max="8" width="17.42578125" style="52" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="52" customWidth="1"/>
+    <col min="1" max="4" width="30.7109375" style="6"/>
+    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="6"/>
+    <col min="8" max="8" width="17.42578125" style="32" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="32" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" style="5"/>
-    <col min="11" max="11" width="26.85546875" style="18" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="14" style="18" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="18" customWidth="1"/>
-    <col min="15" max="15" width="51" style="52" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" style="52" customWidth="1"/>
-    <col min="17" max="17" width="20" style="52" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="18" customWidth="1"/>
-    <col min="19" max="19" width="20.42578125" style="18" customWidth="1"/>
-    <col min="20" max="20" width="21.42578125" style="18" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" style="18" customWidth="1"/>
-    <col min="22" max="16384" width="30.7109375" style="18"/>
+    <col min="11" max="11" width="26.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="14" style="6" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="51" style="32" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" style="32" customWidth="1"/>
+    <col min="17" max="17" width="20" style="32" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="30.7109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="T1" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="50" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="26" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="15"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="50"/>
     </row>
     <row r="3" spans="1:21" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="13">
         <v>1</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>6</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="H4" s="13">
+        <v>2</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>6</v>
+      </c>
+      <c r="R4" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="P3" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="38">
-        <v>6</v>
-      </c>
-      <c r="R3" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="T3" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="U3" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="S4" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="C5" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E5" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="H4" s="33">
-        <v>2</v>
-      </c>
-      <c r="I4" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="36" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="P4" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="38">
-        <v>6</v>
-      </c>
-      <c r="R4" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S4" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T4" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="U4" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="33">
+      <c r="H5" s="13">
         <v>3</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="L5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45" t="s">
+      <c r="M5" s="25"/>
+      <c r="N5" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="18">
         <v>6</v>
       </c>
-      <c r="R5" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S5" s="38" t="s">
+      <c r="R5" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S5" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="U5" s="38" t="s">
-        <v>239</v>
+      <c r="U5" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="H6" s="33">
+      <c r="F6" s="17"/>
+      <c r="G6" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="H6" s="13">
         <v>4</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45" t="s">
+      <c r="M6" s="25"/>
+      <c r="N6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="18">
         <v>6</v>
       </c>
-      <c r="R6" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S6" s="38" t="s">
+      <c r="R6" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S6" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="T6" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="U6" s="38" t="s">
-        <v>239</v>
+      <c r="U6" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="28" t="s">
+      <c r="C7" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="H7" s="33">
+      <c r="F7" s="17"/>
+      <c r="G7" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="13">
         <v>5</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45" t="s">
+      <c r="M7" s="25"/>
+      <c r="N7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="P7" s="37" t="s">
+      <c r="O7" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="P7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7" s="18">
         <v>6</v>
       </c>
-      <c r="R7" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S7" s="38" t="s">
+      <c r="R7" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S7" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T7" s="40" t="s">
+      <c r="T7" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="U7" s="38" t="s">
-        <v>239</v>
+      <c r="U7" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="H8" s="33">
+      <c r="F8" s="17"/>
+      <c r="G8" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="H8" s="13">
         <v>6</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45" t="s">
+      <c r="M8" s="25"/>
+      <c r="N8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="P8" s="37" t="s">
+      <c r="P8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8" s="18">
         <v>6</v>
       </c>
-      <c r="R8" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S8" s="38" t="s">
+      <c r="R8" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S8" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T8" s="40" t="s">
+      <c r="T8" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="U8" s="38" t="s">
-        <v>239</v>
+      <c r="U8" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="42" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="13">
         <v>7</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45" t="s">
+      <c r="M9" s="25"/>
+      <c r="N9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="P9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="18">
         <v>6</v>
       </c>
-      <c r="R9" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S9" s="38" t="s">
+      <c r="R9" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S9" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T9" s="40" t="s">
-        <v>240</v>
-      </c>
-      <c r="U9" s="38" t="s">
-        <v>239</v>
+      <c r="T9" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="42" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="13">
         <v>8</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="23" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="25"/>
+      <c r="O10" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>6</v>
+      </c>
+      <c r="R10" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="K10" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="N10" s="45"/>
-      <c r="O10" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="38">
-        <v>6</v>
-      </c>
-      <c r="R10" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S10" s="38" t="s">
+      <c r="S10" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="T10" s="40" t="s">
+      <c r="T10" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="U10" s="38" t="s">
-        <v>234</v>
+      <c r="U10" s="18" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="H11" s="33">
+      <c r="F11" s="17"/>
+      <c r="G11" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H11" s="13">
         <v>9</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45" t="s">
+      <c r="M11" s="25"/>
+      <c r="N11" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O11" s="36" t="s">
+      <c r="O11" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="P11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>6</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T11" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="H12" s="13">
+        <v>10</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="P11" s="37" t="s">
+      <c r="K12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="P12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q12" s="18">
         <v>6</v>
       </c>
-      <c r="R11" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S11" s="38" t="s">
+      <c r="R12" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S12" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T11" s="40" t="s">
-        <v>241</v>
-      </c>
-      <c r="U11" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="T12" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="U12" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B13" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="42" t="s">
+      <c r="C13" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="13">
+        <v>11</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13" s="25"/>
+      <c r="O13" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="P13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>6</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S13" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="T13" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="H14" s="13">
+        <v>12</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="P14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>6</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S14" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T14" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="H15" s="13">
+        <v>13</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>6</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T15" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="U15" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" s="13">
+        <v>14</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="25"/>
+      <c r="O16" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>6</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S16" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="T16" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="U16" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" s="13">
+        <v>15</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="H12" s="33">
-        <v>10</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K12" s="34" t="s">
+      <c r="K17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L17" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="O12" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="P12" s="37" t="s">
+      <c r="M17" s="25"/>
+      <c r="N17" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="P17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q17" s="18">
         <v>6</v>
       </c>
-      <c r="R12" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S12" s="38" t="s">
+      <c r="R17" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S17" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T12" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="U12" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="T17" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="U17" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="42" t="s">
-        <v>187</v>
-      </c>
-      <c r="H13" s="33">
-        <v>11</v>
-      </c>
-      <c r="I13" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" s="45"/>
-      <c r="O13" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="P13" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="38">
-        <v>6</v>
-      </c>
-      <c r="R13" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S13" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="T13" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="U13" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="H14" s="33">
-        <v>12</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="K14" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="P14" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="38">
-        <v>6</v>
-      </c>
-      <c r="R14" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S14" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T14" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="U14" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="H15" s="33">
-        <v>13</v>
-      </c>
-      <c r="I15" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="K15" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>6</v>
-      </c>
-      <c r="R15" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S15" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T15" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="U15" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="H16" s="33">
-        <v>14</v>
-      </c>
-      <c r="I16" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="K16" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="N16" s="45"/>
-      <c r="O16" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="P16" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="38">
-        <v>6</v>
-      </c>
-      <c r="R16" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S16" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="T16" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="U16" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="H17" s="33">
-        <v>15</v>
-      </c>
-      <c r="I17" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="K17" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="P17" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="38">
-        <v>6</v>
-      </c>
-      <c r="R17" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S17" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T17" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="U17" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E18" s="41" t="s">
+      <c r="C18" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="H18" s="33">
+      <c r="F18" s="17"/>
+      <c r="G18" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="H18" s="13">
         <v>16</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="K18" s="34" t="s">
+      <c r="K18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="44" t="s">
+      <c r="L18" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45" t="s">
+      <c r="M18" s="25"/>
+      <c r="N18" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="36" t="s">
+      <c r="O18" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="P18" s="37" t="s">
+      <c r="P18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="18">
         <v>6</v>
       </c>
-      <c r="R18" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S18" s="38" t="s">
+      <c r="R18" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S18" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T18" s="40" t="s">
+      <c r="T18" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="U18" s="38" t="s">
-        <v>239</v>
+      <c r="U18" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="42" t="s">
+      <c r="C19" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="13">
         <v>17</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="23" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M19" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" s="25"/>
+      <c r="O19" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="K19" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="N19" s="45"/>
-      <c r="O19" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="P19" s="37" t="s">
+      <c r="P19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="18">
         <v>6</v>
       </c>
-      <c r="R19" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S19" s="38" t="s">
+      <c r="R19" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S19" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="T19" s="40" t="s">
-        <v>235</v>
-      </c>
-      <c r="U19" s="38" t="s">
-        <v>234</v>
+      <c r="T19" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="U19" s="18" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E20" s="41" t="s">
+      <c r="C20" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="H20" s="33">
+      <c r="F20" s="17"/>
+      <c r="G20" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20" s="13">
         <v>18</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="23" t="s">
         <v>132</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="L20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45" t="s">
+      <c r="M20" s="25"/>
+      <c r="N20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="P20" s="37" t="s">
+      <c r="O20" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="P20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="38">
+      <c r="Q20" s="18">
         <v>6</v>
       </c>
-      <c r="R20" s="39" t="s">
+      <c r="R20" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S20" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T20" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="U20" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="H21" s="13">
+        <v>19</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>6</v>
+      </c>
+      <c r="R21" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S21" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T21" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="U21" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="H22" s="13">
+        <v>20</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="P22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>6</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S22" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T22" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="S20" s="38" t="s">
+      <c r="U22" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" s="13">
+        <v>21</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="25"/>
+      <c r="O23" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="18">
+        <v>6</v>
+      </c>
+      <c r="R23" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="S23" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="T23" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="U23" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="13">
+        <v>22</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q24" s="18">
+        <v>6</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S24" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="T20" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="U20" s="38" t="s">
+      <c r="T24" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="U24" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="H25" s="13">
+        <v>23</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>6</v>
+      </c>
+      <c r="R25" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T25" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="U25" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" s="13">
+        <v>24</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="18">
+        <v>6</v>
+      </c>
+      <c r="R26" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S26" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T26" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="U26" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="13">
+        <v>25</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="28"/>
+    </row>
+    <row r="28" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="13">
+        <v>26</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q28" s="18">
+        <v>6</v>
+      </c>
+      <c r="R28" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T28" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="U28" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="H29" s="13">
+        <v>27</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="O29" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q29" s="18">
+        <v>6</v>
+      </c>
+      <c r="R29" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="S29" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="T29" s="20" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D21" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" s="33">
-        <v>19</v>
-      </c>
-      <c r="I21" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="K21" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45" t="s">
+      <c r="U29" s="18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="O21" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="P21" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="38">
-        <v>6</v>
-      </c>
-      <c r="R21" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S21" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T21" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="U21" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="H22" s="33">
-        <v>20</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="O22" s="36"/>
-      <c r="P22" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="38">
-        <v>6</v>
-      </c>
-      <c r="R22" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S22" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T22" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="U22" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="47" t="s">
-        <v>207</v>
-      </c>
-      <c r="H23" s="33">
-        <v>21</v>
-      </c>
-      <c r="I23" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="K23" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="M23" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="N23" s="45"/>
-      <c r="O23" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="P23" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="38">
-        <v>6</v>
-      </c>
-      <c r="R23" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="S23" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="T23" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="U23" s="38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="47" t="s">
-        <v>208</v>
-      </c>
-      <c r="H24" s="33">
-        <v>22</v>
-      </c>
-      <c r="I24" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="K24" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="36" t="s">
-        <v>210</v>
-      </c>
-      <c r="P24" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q24" s="38">
-        <v>6</v>
-      </c>
-      <c r="R24" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S24" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T24" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="U24" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="H25" s="33">
-        <v>23</v>
-      </c>
-      <c r="I25" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="O25" s="36"/>
-      <c r="P25" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="38">
-        <v>6</v>
-      </c>
-      <c r="R25" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S25" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T25" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="U25" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="H26" s="33">
-        <v>24</v>
-      </c>
-      <c r="I26" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="K26" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O26" s="36" t="s">
-        <v>211</v>
-      </c>
-      <c r="P26" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="38">
-        <v>6</v>
-      </c>
-      <c r="R26" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S26" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T26" s="40" t="s">
-        <v>242</v>
-      </c>
-      <c r="U26" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D27" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="33">
-        <v>25</v>
-      </c>
-      <c r="I27" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="K27" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="48"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="48"/>
-    </row>
-    <row r="28" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D28" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="H28" s="33">
-        <v>26</v>
-      </c>
-      <c r="I28" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="K28" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="O28" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="P28" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q28" s="38">
-        <v>6</v>
-      </c>
-      <c r="R28" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S28" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T28" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="U28" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="H29" s="33">
-        <v>27</v>
-      </c>
-      <c r="I29" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="K29" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="O29" s="51" t="s">
-        <v>222</v>
-      </c>
-      <c r="P29" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="38">
-        <v>6</v>
-      </c>
-      <c r="R29" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="S29" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="T29" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="U29" s="38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="18" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="76" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="6" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3312,12 +3328,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>